<commit_message>
download file API Created
</commit_message>
<xml_diff>
--- a/studentData.xlsx
+++ b/studentData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,117 @@
   </si>
   <si>
     <t>24/3/2025, 7:00:56 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:04:19 pm</t>
+  </si>
+  <si>
+    <t>In a month</t>
+  </si>
+  <si>
+    <t>dfsd</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:27:40 pm</t>
+  </si>
+  <si>
+    <t>Basic Web Designing</t>
+  </si>
+  <si>
+    <t>wedwe</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:28:24 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:28:35 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:29:09 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:31:24 pm</t>
+  </si>
+  <si>
+    <t>Rahul Singh Chouhan</t>
+  </si>
+  <si>
+    <t>citstedev@gmail.com</t>
+  </si>
+  <si>
+    <t>Cake PHP</t>
+  </si>
+  <si>
+    <t>This Week</t>
+  </si>
+  <si>
+    <t>hy</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:31:29 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:37:25 pm</t>
+  </si>
+  <si>
+    <t>cits dev</t>
+  </si>
+  <si>
+    <t>C, C++ with Data Structure</t>
+  </si>
+  <si>
+    <t>fghghfg</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:37:54 pm</t>
+  </si>
+  <si>
+    <t>fddfd</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:38:12 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:39:08 pm</t>
+  </si>
+  <si>
+    <t>wdwedwe</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:40:03 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:40:16 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:40:23 pm</t>
+  </si>
+  <si>
+    <t>24/3/2025, 7:40:31 pm</t>
+  </si>
+  <si>
+    <t>25/3/2025, 10:24:05 am</t>
+  </si>
+  <si>
+    <t>fsdfsds</t>
+  </si>
+  <si>
+    <t>25/3/2025, 10:24:13 am</t>
+  </si>
+  <si>
+    <t>25/3/2025, 10:24:19 am</t>
+  </si>
+  <si>
+    <t>25/3/2025, 10:47:59 am</t>
+  </si>
+  <si>
+    <t>25/3/2025, 10:49:39 am</t>
+  </si>
+  <si>
+    <t>25/3/2025, 1:06:19 pm</t>
+  </si>
+  <si>
+    <t>dsafsdafe</t>
   </si>
 </sst>
 </file>
@@ -451,7 +562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -578,6 +689,489 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>2342342342</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>2342342342</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>2342342342</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>2342342342</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>2342342342</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>2342342342</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>2342342342</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>2342342342</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>2342342342</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>2342342342</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>2342342342</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>2342342342</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>2342342342</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>2342342342</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>2342342342</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>2342342342</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>2342342342</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <v>2342342342</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>2342342342</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <v>2342342342</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" ht="25" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>2342342342</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>